<commit_message>
Added EDA for subindexes
</commit_message>
<xml_diff>
--- a/data/cpi.xlsx
+++ b/data/cpi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\работа\Крушинина графики для сайта\2021\04 апрель\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\работа\Крушинина графики для сайта\2021\05 май\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -196,7 +196,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">Апрель 2021 г. в % к декабрю 2020 г.
+      <t xml:space="preserve">Май 2021 г. в % к декабрю 2020 г.
        Руководствуясь теорией статистики, для получения ИПЦ за произвольный период необходимо перемножить все входящие в этот временной промежуток индексы, характеризующие изменение цен в отчетном периоде по сравнению с предыдущим. Так, например, индекс потребительских цен по Российской Федерации за период 
 январь 2020 г. - апрель 2020 г. рассчитывается следующим образом:
                                                                                         100,40 * 100,33 : 100 * 100,55 : 100 * 100,83 : 100 = 102,13%
@@ -228,7 +228,7 @@
   </si>
   <si>
     <r>
-      <t>102,72</t>
+      <t>103,48</t>
     </r>
     <r>
       <rPr>
@@ -919,7 +919,7 @@
   <dimension ref="A1:AI20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:AF20"/>
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1653,7 +1653,9 @@
       <c r="AE10" s="25">
         <v>100.27</v>
       </c>
-      <c r="AF10" s="25"/>
+      <c r="AF10" s="25">
+        <v>100.74</v>
+      </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">

</xml_diff>